<commit_message>
New code for extracting description from website
</commit_message>
<xml_diff>
--- a/daft_listings_with_coordinates.xlsx
+++ b/daft_listings_with_coordinates.xlsx
@@ -468,169 +468,169 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>One Lime Street, Docklands, Dublin 2</t>
+          <t>Monkstown Grove , Monkstown Grove , Monkstown, Co. Dublin</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>One Lime Street, Docklands, Dublin 2</t>
+          <t>Monkstown Grove , Monkstown Grove , Monkstown, Co. Dublin</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2400</v>
+        <v>1975</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>53.34551330632709</v>
+        <v>53.28617687295534</v>
       </c>
       <c r="F2" t="n">
-        <v>-6.243459428241323</v>
+        <v>-6.155262552390525</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Occu East Village, Leopardstown, Dublin 18, Clay Farm Drive, Leopardstown, Dublin 18</t>
+          <t>St Edmunds Avenue , St Edmunds Avenue , Lucan, Co. Dublin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Occu East Village, Leopardstown, Dublin 18, Clay Farm Drive, Leopardstown, Dublin 18</t>
+          <t>St Edmunds Avenue , St Edmunds Avenue , Lucan, Co. Dublin</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2150</v>
+        <v>1975</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>53.25557244538155</v>
+        <v>53.3539171471368</v>
       </c>
       <c r="F3" t="n">
-        <v>-6.201061947657053</v>
+        <v>-6.406624739021879</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Quayside Quarter, North Wall Quay, Dublin 1</t>
+          <t>One Lime Street, Docklands, Dublin 2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Quayside Quarter, North Wall Quay, Dublin 1</t>
+          <t>One Lime Street, Docklands, Dublin 2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2517</v>
+        <v>2400</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>53.34747481688501</v>
+        <v>53.34551330632709</v>
       </c>
       <c r="F4" t="n">
-        <v>-6.233233248674509</v>
+        <v>-6.243459428241323</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Grand Canal Harbour, Grand Canal Place, Dublin 8</t>
+          <t>Occu East Village, Leopardstown, Dublin 18, Clay Farm Drive, Leopardstown, Dublin 18</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Grand Canal Harbour, Grand Canal Place, Dublin 8</t>
+          <t>Occu East Village, Leopardstown, Dublin 18, Clay Farm Drive, Leopardstown, Dublin 18</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>2150</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>53.3418330178848</v>
+        <v>53.25557244538155</v>
       </c>
       <c r="F5" t="n">
-        <v>-6.288615427057721</v>
+        <v>-6.201061947657053</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sandford Lodge, Sandford Lodge, Ranelagh, Dublin 6, Ranelagh, Dublin 6</t>
+          <t>Quayside Quarter, North Wall Quay, Dublin 1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sandford Lodge, Sandford Lodge, Ranelagh, Dublin 6, Ranelagh, Dublin 6</t>
+          <t>Quayside Quarter, North Wall Quay, Dublin 1</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4000</v>
+        <v>2517</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>53.3193336810545</v>
+        <v>53.34747481688501</v>
       </c>
       <c r="F6" t="n">
-        <v>-6.248271768122493</v>
+        <v>-6.233233248674509</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cathedral Court, Unit 6 New Street South, Dublin 8</t>
+          <t>Grand Canal Harbour, Grand Canal Place, Dublin 8</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cathedral Court, Unit 6 New Street South, Dublin 8</t>
+          <t>Grand Canal Harbour, Grand Canal Place, Dublin 8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2991</v>
+        <v>2150</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>53.33739010497453</v>
+        <v>53.3418330178848</v>
       </c>
       <c r="F7" t="n">
-        <v>-6.272850320541352</v>
+        <v>-6.288615427057721</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spencer Place, Spencer Place, Dublin 1</t>
+          <t>Sandford Lodge, Sandford Lodge, Ranelagh, Dublin 6, Ranelagh, Dublin 6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Spencer Place, Spencer Place, Dublin 1</t>
+          <t>Sandford Lodge, Sandford Lodge, Ranelagh, Dublin 6, Ranelagh, Dublin 6</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2125</v>
+        <v>4000</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>53.34948314901089</v>
+        <v>53.3193336810545</v>
       </c>
       <c r="F8" t="n">
-        <v>-6.235875899678973</v>
+        <v>-6.248271768122493</v>
       </c>
     </row>
     <row r="9">
@@ -660,73 +660,73 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>The Lookout , Harbour Road, Dalkey, Co. Dublin</t>
+          <t>Spencer Place, Spencer Place, Dublin 1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>The Lookout , Harbour Road, Dalkey, Co. Dublin</t>
+          <t>Spencer Place, Spencer Place, Dublin 1</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2150</v>
+        <v>2125</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>53.28090230919184</v>
+        <v>53.34948314901089</v>
       </c>
       <c r="F10" t="n">
-        <v>-6.102395690038719</v>
+        <v>-6.235875899678973</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Green Acre Grange , Upper Kilmacud Road , Dundrum, Dublin 14</t>
+          <t>The Lookout , Harbour Road, Dalkey, Co. Dublin</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Green Acre Grange , Upper Kilmacud Road , Dundrum, Dublin 14</t>
+          <t>The Lookout , Harbour Road, Dalkey, Co. Dublin</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2050</v>
+        <v>2150</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>53.28906080866142</v>
+        <v>53.28090230919184</v>
       </c>
       <c r="F11" t="n">
-        <v>-6.233999498080863</v>
+        <v>-6.102395690038719</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>O'Callaghan Court , Erne Street Upper , Dublin 2</t>
+          <t>Green Acre Grange , Upper Kilmacud Road , Dundrum, Dublin 14</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>O'Callaghan Court , Erne Street Upper , Dublin 2</t>
+          <t>Green Acre Grange , Upper Kilmacud Road , Dundrum, Dublin 14</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2450</v>
+        <v>2050</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>53.34185191360561</v>
+        <v>53.28906080866142</v>
       </c>
       <c r="F12" t="n">
-        <v>-6.245194894252535</v>
+        <v>-6.233999498080863</v>
       </c>
     </row>
     <row r="13">
@@ -804,145 +804,145 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>8th Lock , Ratoath Road, Ashtown , Dublin 11</t>
+          <t>O'Callaghan Court , Erne Street Upper , Dublin 2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>8th Lock , Ratoath Road, Ashtown , Dublin 11</t>
+          <t>O'Callaghan Court , Erne Street Upper , Dublin 2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1900</v>
+        <v>2450</v>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>53.3753383143067</v>
+        <v>53.34185191360561</v>
       </c>
       <c r="F16" t="n">
-        <v>-6.309066266937265</v>
+        <v>-6.245194894252535</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Barnoaks, The Green, Citywest, Co. Dublin</t>
+          <t>Cathedral Court, Unit 6 New Street South, Dublin 8</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Barnoaks, The Green, Citywest, Co. Dublin</t>
+          <t>Cathedral Court, Unit 6 New Street South, Dublin 8</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1925</v>
+        <v>2991</v>
       </c>
       <c r="D17" t="n">
         <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>53.28005835188762</v>
+        <v>53.33739010497453</v>
       </c>
       <c r="F17" t="n">
-        <v>-6.420131669334353</v>
+        <v>-6.272850320541352</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Two Oaks , Scholarstown Road , Knocklyon, Dublin 16</t>
+          <t>8th Lock , Ratoath Road, Ashtown , Dublin 11</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Two Oaks , Scholarstown Road , Knocklyon, Dublin 16</t>
+          <t>8th Lock , Ratoath Road, Ashtown , Dublin 11</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1875</v>
+        <v>1900</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>53.27934714613909</v>
+        <v>53.3753383143067</v>
       </c>
       <c r="F18" t="n">
-        <v>-6.313134063107952</v>
+        <v>-6.309066266937265</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>St Edmunds Avenue , St Edmunds Avenue , Lucan, Co. Dublin</t>
+          <t xml:space="preserve"> Barnoaks, The Green, Citywest, Co. Dublin</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>St Edmunds Avenue , St Edmunds Avenue , Lucan, Co. Dublin</t>
+          <t xml:space="preserve"> Barnoaks, The Green, Citywest, Co. Dublin</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1875</v>
+        <v>1925</v>
       </c>
       <c r="D19" t="n">
         <v>3</v>
       </c>
       <c r="E19" t="n">
-        <v>53.3539171471368</v>
+        <v>53.28005835188762</v>
       </c>
       <c r="F19" t="n">
-        <v>-6.406624739021879</v>
+        <v>-6.420131669334353</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Station View , The Crossings , Adamstown, Co. Dublin</t>
+          <t>Two Oaks , Scholarstown Road , Knocklyon, Dublin 16</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Station View , The Crossings , Adamstown, Co. Dublin</t>
+          <t>Two Oaks , Scholarstown Road , Knocklyon, Dublin 16</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1725</v>
+        <v>1875</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>53.33654749096823</v>
+        <v>53.27934714613909</v>
       </c>
       <c r="F20" t="n">
-        <v>-6.4696388950901</v>
+        <v>-6.313134063107952</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Seafield Strand, Greenfield Road, Sutton, Dublin 13</t>
+          <t>Kilcarbery Square , Kilcarbery Grange , Clondalkin, Dublin 22</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Seafield Strand, Greenfield Road, Sutton, Dublin 13</t>
+          <t>Kilcarbery Square , Kilcarbery Grange , Clondalkin, Dublin 22</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2150</v>
+        <v>1925</v>
       </c>
       <c r="D21" t="n">
         <v>3</v>
       </c>
       <c r="E21" t="n">
-        <v>53.38693545299904</v>
+        <v>53.31427821306829</v>
       </c>
       <c r="F21" t="n">
-        <v>-6.10259279972712</v>
+        <v>-6.425069126931987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>